<commit_message>
added adversarial models inpainting vase + kate got better results than regular training
</commit_message>
<xml_diff>
--- a/experiments/experiments_results.xlsx
+++ b/experiments/experiments_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aviv_\Documents\DeepImagePriorProject\experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{994D41CB-FF50-4D9E-B3F1-EF26F779AAF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86495F0F-3119-4388-9A45-ADA87132F18B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C50AFBCF-CB5F-478B-8ACE-8DDE4907E3C8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t xml:space="preserve">IMAGE - MODEL </t>
   </si>
@@ -77,26 +77,41 @@
     <t>library - fixed dsc deep - adversarial</t>
   </si>
   <si>
-    <t>library - deep dsc like downsacler - adversarial</t>
-  </si>
-  <si>
-    <t>not good</t>
-  </si>
-  <si>
-    <t>kate - fixed dsc deep - adversarial</t>
-  </si>
-  <si>
     <t>barabara - fixed deep dsc - adversarial</t>
   </si>
   <si>
     <t>need to run a few times to find good starting point</t>
+  </si>
+  <si>
+    <t>kate - fixed deep dsc - adversarial</t>
+  </si>
+  <si>
+    <t>much more stable than before</t>
+  </si>
+  <si>
+    <t>much better, converge much faster and better results</t>
+  </si>
+  <si>
+    <t>much better than before even better than normal training</t>
+  </si>
+  <si>
+    <t>kate - fixed dsc deep adversarial</t>
+  </si>
+  <si>
+    <t>much faster</t>
+  </si>
+  <si>
+    <t>poor looking results probably because gen_lr too small</t>
+  </si>
+  <si>
+    <t>better than regular training</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -107,6 +122,13 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
@@ -134,9 +156,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98309F2E-959E-41C5-8EA8-D487D0259B9F}">
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="H50" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -513,7 +536,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="H3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -587,278 +610,512 @@
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>21.65</v>
+      </c>
+      <c r="C8">
+        <v>57.24</v>
+      </c>
+      <c r="E8">
+        <v>19000</v>
+      </c>
+      <c r="F8">
+        <v>1E-4</v>
+      </c>
+      <c r="G8">
+        <v>1E-4</v>
+      </c>
+      <c r="H8" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>16</v>
-      </c>
       <c r="B9">
-        <v>25.6</v>
+        <v>23.58</v>
       </c>
       <c r="C9">
-        <v>31.26</v>
+        <v>61.88</v>
       </c>
       <c r="E9">
-        <v>6000</v>
+        <v>9900</v>
       </c>
       <c r="F9">
-        <v>7.4999999999999997E-3</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="G9">
-        <v>5.0000000000000001E-3</v>
+        <v>1E-4</v>
+      </c>
+      <c r="H9" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B10">
-        <v>26.5</v>
+        <v>23.76</v>
       </c>
       <c r="C10">
-        <v>37.200000000000003</v>
+        <v>61.23</v>
       </c>
       <c r="E10">
-        <v>15000</v>
+        <v>16450</v>
       </c>
       <c r="F10">
-        <v>7.4999999999999997E-3</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="G10">
-        <v>5.0000000000000001E-3</v>
+        <v>1E-4</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B11">
-        <v>28.3</v>
+        <v>23.81</v>
       </c>
       <c r="C11">
-        <v>40.119999999999997</v>
+        <v>53.2</v>
       </c>
       <c r="E11">
-        <v>22800</v>
+        <v>2150</v>
       </c>
       <c r="F11">
         <v>1E-3</v>
       </c>
       <c r="G11">
-        <v>1E-3</v>
+        <v>1E-4</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B12">
+        <v>24.04</v>
+      </c>
+      <c r="C12">
+        <v>58.8</v>
+      </c>
+      <c r="E12">
+        <v>4600</v>
+      </c>
+      <c r="F12">
+        <v>1E-3</v>
+      </c>
+      <c r="G12">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="1">
+        <v>24.36</v>
+      </c>
+      <c r="C13">
+        <v>63.34</v>
+      </c>
+      <c r="E13">
+        <v>16550</v>
+      </c>
+      <c r="F13">
+        <v>1E-3</v>
+      </c>
+      <c r="G13">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>25.6</v>
+      </c>
+      <c r="C17">
+        <v>31.26</v>
+      </c>
+      <c r="E17">
+        <v>6000</v>
+      </c>
+      <c r="F17">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="G17">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>26.5</v>
+      </c>
+      <c r="C18">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="E18">
+        <v>15000</v>
+      </c>
+      <c r="F18">
+        <v>7.4999999999999997E-3</v>
+      </c>
+      <c r="G18">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>28.3</v>
+      </c>
+      <c r="C19">
+        <v>40.119999999999997</v>
+      </c>
+      <c r="E19">
+        <v>22800</v>
+      </c>
+      <c r="F19">
+        <v>1E-3</v>
+      </c>
+      <c r="G19">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B20" s="1">
         <v>29.09</v>
       </c>
-      <c r="E12">
+      <c r="E20">
         <v>30000</v>
       </c>
-      <c r="F12">
-        <v>1E-3</v>
-      </c>
-      <c r="G12">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="F20">
+        <v>1E-3</v>
+      </c>
+      <c r="G20">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
         <v>11</v>
       </c>
-      <c r="B17">
+      <c r="B25">
         <v>19.98</v>
       </c>
-      <c r="E17">
+      <c r="E25">
         <v>5000</v>
       </c>
-      <c r="F17">
+      <c r="F25">
         <v>0.01</v>
       </c>
-      <c r="G17">
+      <c r="G25">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B18">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B26">
         <v>18.7</v>
       </c>
-      <c r="C18">
+      <c r="C26">
         <v>19.149999999999999</v>
       </c>
-      <c r="E18">
+      <c r="E26">
         <v>5000</v>
       </c>
-      <c r="F18">
+      <c r="F26">
         <v>0.01</v>
       </c>
-      <c r="G18">
+      <c r="G26">
         <v>0.01</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B19">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B27">
         <v>18.920000000000002</v>
       </c>
-      <c r="C19">
+      <c r="C27">
         <v>19.489999999999998</v>
       </c>
-      <c r="E19">
+      <c r="E27">
         <v>4700</v>
       </c>
-      <c r="F19">
+      <c r="F27">
         <v>0.01</v>
       </c>
-      <c r="G19">
+      <c r="G27">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B20">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B28">
         <v>21.57</v>
       </c>
-      <c r="C20">
+      <c r="C28">
         <v>22.73</v>
       </c>
-      <c r="E20">
+      <c r="E28">
         <v>10000</v>
       </c>
-      <c r="F20">
+      <c r="F28">
         <v>0.01</v>
       </c>
-      <c r="G20">
+      <c r="G28">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B21">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B29" s="2">
         <v>26.33</v>
       </c>
-      <c r="C21">
+      <c r="C29">
         <v>29.37</v>
       </c>
-      <c r="E21">
+      <c r="E29">
         <v>12850</v>
       </c>
-      <c r="F21">
+      <c r="F29">
         <v>0.01</v>
       </c>
-      <c r="G21">
+      <c r="G29">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B30" s="2">
+        <v>29.19</v>
+      </c>
+      <c r="C30">
+        <v>37.29</v>
+      </c>
+      <c r="E30">
+        <v>6200</v>
+      </c>
+      <c r="F30">
+        <v>1E-3</v>
+      </c>
+      <c r="G30">
+        <v>1E-4</v>
+      </c>
+      <c r="H30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B31" s="1">
+        <v>29.88</v>
+      </c>
+      <c r="C31">
+        <v>40.950000000000003</v>
+      </c>
+      <c r="E31">
+        <v>18000</v>
+      </c>
+      <c r="F31">
+        <v>1E-3</v>
+      </c>
+      <c r="G31">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
         <v>12</v>
       </c>
-      <c r="B23">
+      <c r="B37">
         <v>16.25</v>
       </c>
-      <c r="C23">
+      <c r="C37">
         <v>21.6</v>
       </c>
-      <c r="E23">
+      <c r="E37">
         <v>12950</v>
       </c>
-      <c r="F23">
+      <c r="F37">
         <v>0.01</v>
       </c>
-      <c r="G23">
+      <c r="G37">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B24">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B38">
         <v>16.37</v>
       </c>
-      <c r="C24">
+      <c r="C38">
         <v>21.7</v>
       </c>
-      <c r="E24">
+      <c r="E38">
         <v>21000</v>
       </c>
-      <c r="F24">
+      <c r="F38">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="G24">
+      <c r="G38">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B25">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B39" s="1">
         <v>16.600000000000001</v>
       </c>
-      <c r="C25">
+      <c r="C39">
         <v>21.08</v>
       </c>
-      <c r="E25">
+      <c r="E39">
         <v>9850</v>
       </c>
-      <c r="F25">
+      <c r="F39">
         <v>7.4999999999999997E-3</v>
       </c>
-      <c r="G25">
+      <c r="G39">
         <v>5.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B26">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B40">
         <v>16.059999999999999</v>
       </c>
-      <c r="C26">
+      <c r="C40">
         <v>20</v>
       </c>
-      <c r="E26">
+      <c r="E40">
         <v>8400</v>
       </c>
-      <c r="F26">
+      <c r="F40">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="G26">
+      <c r="G40">
         <v>3.0000000000000001E-3</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>13</v>
-      </c>
-      <c r="B30" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>15</v>
-      </c>
-      <c r="B32">
-        <v>31</v>
-      </c>
-      <c r="C32">
-        <v>32</v>
-      </c>
-      <c r="E32">
-        <v>15500</v>
-      </c>
-      <c r="F32">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="G32">
-        <v>5.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="33" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B33">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <v>16.54</v>
+      </c>
+      <c r="C41">
+        <v>21.5</v>
+      </c>
+      <c r="E41">
+        <v>4250</v>
+      </c>
+      <c r="F41">
+        <v>1E-3</v>
+      </c>
+      <c r="G41">
+        <v>1E-4</v>
+      </c>
+      <c r="H41" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B42">
+        <v>16.55</v>
+      </c>
+      <c r="C42">
+        <v>22.6</v>
+      </c>
+      <c r="E42">
+        <v>2800</v>
+      </c>
+      <c r="F42">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G42">
+        <v>5.0000000000000002E-5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B43">
+        <v>17</v>
+      </c>
+      <c r="C43">
+        <v>23.69</v>
+      </c>
+      <c r="E43">
+        <v>9600</v>
+      </c>
+      <c r="F43">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="G43">
+        <v>5.0000000000000002E-5</v>
+      </c>
+      <c r="H43" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" s="2">
         <v>32.83</v>
       </c>
-      <c r="C33">
+      <c r="C47">
         <v>33.520000000000003</v>
       </c>
-      <c r="E33">
+      <c r="E47">
         <v>14200</v>
       </c>
-      <c r="F33">
+      <c r="F47">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="G33">
+      <c r="G47">
         <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B48">
+        <v>38</v>
+      </c>
+      <c r="C48">
+        <v>40</v>
+      </c>
+      <c r="E48">
+        <v>4650</v>
+      </c>
+      <c r="F48">
+        <v>1E-3</v>
+      </c>
+      <c r="G48">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B49">
+        <v>39.47</v>
+      </c>
+      <c r="C49">
+        <v>42</v>
+      </c>
+      <c r="E49">
+        <v>16650</v>
+      </c>
+      <c r="F49">
+        <v>1E-3</v>
+      </c>
+      <c r="G49">
+        <v>1E-4</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B50" s="1">
+        <v>39.75</v>
+      </c>
+      <c r="C50">
+        <v>42.5</v>
+      </c>
+      <c r="E50">
+        <v>19000</v>
+      </c>
+      <c r="F50">
+        <v>1E-3</v>
+      </c>
+      <c r="G50">
+        <v>1E-4</v>
+      </c>
+      <c r="H50" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleaned some notebooks, and added all notebooks restult - images and graphs
</commit_message>
<xml_diff>
--- a/experiments/experiments_results.xlsx
+++ b/experiments/experiments_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aviv_\Documents\DeepImagePriorProject\experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86495F0F-3119-4388-9A45-ADA87132F18B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7601F9CA-A02B-4760-973D-48164188E80F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C50AFBCF-CB5F-478B-8ACE-8DDE4907E3C8}"/>
   </bookViews>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
   <si>
     <t xml:space="preserve">IMAGE - MODEL </t>
   </si>
   <si>
-    <t>loss</t>
-  </si>
-  <si>
     <t>pnsr-masked</t>
   </si>
   <si>
@@ -105,6 +102,66 @@
   </si>
   <si>
     <t>better than regular training</t>
+  </si>
+  <si>
+    <t xml:space="preserve">training with input optim as well </t>
+  </si>
+  <si>
+    <t>adversarial + input optim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">denoising </t>
+  </si>
+  <si>
+    <t>snail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">results </t>
+  </si>
+  <si>
+    <t>kate - regular</t>
+  </si>
+  <si>
+    <t>input - optim</t>
+  </si>
+  <si>
+    <t>adversarial</t>
+  </si>
+  <si>
+    <t>barbara - regular</t>
+  </si>
+  <si>
+    <t>vase - regular</t>
+  </si>
+  <si>
+    <t>library - regular</t>
+  </si>
+  <si>
+    <t>denoising</t>
+  </si>
+  <si>
+    <t>snail - regular</t>
+  </si>
+  <si>
+    <t>jet - regular</t>
+  </si>
+  <si>
+    <t>sr</t>
+  </si>
+  <si>
+    <t>zebra factor 4 - regular</t>
+  </si>
+  <si>
+    <t>zebra factor 8 - regular</t>
+  </si>
+  <si>
+    <t>psnr_masked</t>
+  </si>
+  <si>
+    <t>num_iter</t>
+  </si>
+  <si>
+    <t>worst looking results</t>
   </si>
 </sst>
 </file>
@@ -474,10 +531,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98309F2E-959E-41C5-8EA8-D487D0259B9F}">
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:H103"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="H50" sqref="H50"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -485,6 +542,7 @@
     <col min="1" max="1" width="27.08203125" customWidth="1"/>
     <col min="2" max="3" width="12.1640625" customWidth="1"/>
     <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="17.6640625" customWidth="1"/>
     <col min="8" max="8" width="21.25" customWidth="1"/>
   </cols>
   <sheetData>
@@ -493,32 +551,29 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
         <v>8</v>
-      </c>
-      <c r="G1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>21.17</v>
@@ -536,12 +591,12 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="H3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>17.89</v>
@@ -612,7 +667,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>21.65</v>
@@ -630,7 +685,7 @@
         <v>1E-4</v>
       </c>
       <c r="H8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -650,7 +705,7 @@
         <v>1E-4</v>
       </c>
       <c r="H9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -723,7 +778,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B17">
         <v>25.6</v>
@@ -791,12 +846,12 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B25">
         <v>19.98</v>
@@ -896,18 +951,18 @@
         <v>1E-4</v>
       </c>
       <c r="H30" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B31" s="1">
-        <v>29.88</v>
+        <v>30</v>
       </c>
       <c r="C31">
         <v>40.950000000000003</v>
       </c>
       <c r="E31">
-        <v>18000</v>
+        <v>6000</v>
       </c>
       <c r="F31">
         <v>1E-3</v>
@@ -918,7 +973,7 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B37">
         <v>16.25</v>
@@ -1004,7 +1059,7 @@
         <v>1E-4</v>
       </c>
       <c r="H41" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.3">
@@ -1041,12 +1096,12 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="H43" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B47" s="2">
         <v>32.83</v>
@@ -1081,7 +1136,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B49">
         <v>39.47</v>
       </c>
@@ -1098,7 +1153,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B50" s="1">
         <v>39.75</v>
       </c>
@@ -1115,7 +1170,452 @@
         <v>1E-4</v>
       </c>
       <c r="H50" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>23</v>
+      </c>
+      <c r="B51" s="1">
+        <v>40.82</v>
+      </c>
+      <c r="C51">
+        <v>43</v>
+      </c>
+      <c r="E51">
+        <v>19400</v>
+      </c>
+      <c r="F51">
+        <v>1E-3</v>
+      </c>
+      <c r="G51">
+        <v>1E-4</v>
+      </c>
+      <c r="H51" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>25</v>
+      </c>
+      <c r="B55">
+        <v>20.52</v>
+      </c>
+      <c r="E55">
+        <v>8250</v>
+      </c>
+      <c r="F55">
+        <v>1E-3</v>
+      </c>
+      <c r="G55">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>26</v>
+      </c>
+      <c r="B64" t="s">
+        <v>2</v>
+      </c>
+      <c r="C64" t="s">
+        <v>39</v>
+      </c>
+      <c r="D64" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>27</v>
+      </c>
+      <c r="B66">
+        <v>24.75</v>
+      </c>
+      <c r="C66">
+        <v>48.44</v>
+      </c>
+      <c r="D66">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>28</v>
+      </c>
+      <c r="B67">
+        <v>25.01</v>
+      </c>
+      <c r="C67">
+        <v>48.77</v>
+      </c>
+      <c r="D67">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>29</v>
+      </c>
+      <c r="B68">
+        <v>24.04</v>
+      </c>
+      <c r="C68">
+        <v>58.8</v>
+      </c>
+      <c r="D68">
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>30</v>
+      </c>
+      <c r="B70">
+        <v>32.119999999999997</v>
+      </c>
+      <c r="C70">
+        <v>41.23</v>
+      </c>
+      <c r="D70">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>28</v>
+      </c>
+      <c r="B71">
+        <v>29.66</v>
+      </c>
+      <c r="C71">
+        <v>44.75</v>
+      </c>
+      <c r="D71">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>29</v>
+      </c>
+      <c r="B72">
+        <v>28.3</v>
+      </c>
+      <c r="C72">
+        <v>40.119999999999997</v>
+      </c>
+      <c r="D72">
+        <v>22000</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>27</v>
+      </c>
+      <c r="B75">
+        <v>38.74</v>
+      </c>
+      <c r="C75">
+        <v>39.89</v>
+      </c>
+      <c r="D75">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>28</v>
+      </c>
+      <c r="B76">
+        <v>42.27</v>
+      </c>
+      <c r="C76">
+        <v>49.28</v>
+      </c>
+      <c r="D76">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>29</v>
+      </c>
+      <c r="B77">
+        <v>39.75</v>
+      </c>
+      <c r="C77">
+        <v>42.5</v>
+      </c>
+      <c r="D77">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>31</v>
+      </c>
+      <c r="B79">
+        <v>29.22</v>
+      </c>
+      <c r="C79">
+        <v>35.99</v>
+      </c>
+      <c r="D79">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>28</v>
+      </c>
+      <c r="B80">
+        <v>28.86</v>
+      </c>
+      <c r="C80">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="D80">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>29</v>
+      </c>
+      <c r="B81">
+        <v>30</v>
+      </c>
+      <c r="C81">
+        <v>41</v>
+      </c>
+      <c r="D81">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>32</v>
+      </c>
+      <c r="B83">
+        <v>19.43</v>
+      </c>
+      <c r="C83">
+        <v>29.53</v>
+      </c>
+      <c r="D83">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>28</v>
+      </c>
+      <c r="B84">
+        <v>19.170000000000002</v>
+      </c>
+      <c r="C84">
+        <v>28.85</v>
+      </c>
+      <c r="D84">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>29</v>
+      </c>
+      <c r="B85">
+        <v>16.8</v>
+      </c>
+      <c r="C85">
+        <v>23</v>
+      </c>
+      <c r="D85">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>34</v>
+      </c>
+      <c r="B88">
+        <v>26.51</v>
+      </c>
+      <c r="D88">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>28</v>
+      </c>
+      <c r="B89">
+        <v>29.01</v>
+      </c>
+      <c r="D89">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>29</v>
+      </c>
+      <c r="B90">
+        <v>18.21</v>
+      </c>
+      <c r="D90">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>35</v>
+      </c>
+      <c r="B92">
+        <v>31.6</v>
+      </c>
+      <c r="C92">
+        <v>27.54</v>
+      </c>
+      <c r="D92">
+        <v>2400</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>28</v>
+      </c>
+      <c r="B93">
+        <v>35.229999999999997</v>
+      </c>
+      <c r="C93">
+        <v>29.31</v>
+      </c>
+      <c r="D93">
+        <v>2400</v>
+      </c>
+      <c r="E93" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>29</v>
+      </c>
+      <c r="B94">
+        <v>19</v>
+      </c>
+      <c r="C94">
+        <v>18.87</v>
+      </c>
+      <c r="D94">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A96" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>37</v>
+      </c>
+      <c r="B97">
+        <v>24.03</v>
+      </c>
+      <c r="C97">
+        <v>32.83</v>
+      </c>
+      <c r="D97">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>28</v>
+      </c>
+      <c r="B98">
+        <v>23</v>
+      </c>
+      <c r="C98">
+        <v>43</v>
+      </c>
+      <c r="D98">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>29</v>
+      </c>
+      <c r="D99">
+        <v>1800</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>38</v>
+      </c>
+      <c r="B101">
+        <v>19.54</v>
+      </c>
+      <c r="C101">
+        <v>42.12</v>
+      </c>
+      <c r="D101">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>28</v>
+      </c>
+      <c r="B102">
+        <v>19.12</v>
+      </c>
+      <c r="C102">
+        <v>57.19</v>
+      </c>
+      <c r="D102">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>29</v>
+      </c>
+      <c r="B103">
+        <v>17.93</v>
+      </c>
+      <c r="C103">
+        <v>35.56</v>
+      </c>
+      <c r="D103">
+        <v>4000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>